<commit_message>
Rest Assured - Code Addition
</commit_message>
<xml_diff>
--- a/files/Data.xlsx
+++ b/files/Data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a99afbbb90a07868/Desktop/Project_SDET/Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a99afbbb90a07868/Desktop/Project_SDET/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_F25DC773A252ABDACC10482B719B56585BDE58E4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C10D7E0F-E1E8-4D5D-BCD4-29CF29774011}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_F25DC773A252ABDACC10482B719B56585BDE58E4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{218B8478-8461-4CB0-87C9-5214E6C925B0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -49,16 +50,36 @@
   </si>
   <si>
     <t>Python</t>
+  </si>
+  <si>
+    <t>bhirwe@gmail.com</t>
+  </si>
+  <si>
+    <t>Quick@890</t>
+  </si>
+  <si>
+    <t>eve.holt@reqres.in</t>
+  </si>
+  <si>
+    <t>pistol</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -81,13 +102,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -101,6 +125,14 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -368,7 +400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -410,4 +442,40 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DEEF0A7-B798-49A8-98D8-FDBA8A44A068}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{13C91D5A-1CF9-4056-9502-1CFFAA8131A0}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{2A1EA0DE-02BD-4F82-B865-3F3E4DF8D362}"/>
+    <hyperlink ref="A1" r:id="rId3" xr:uid="{C604ED6A-E6D1-47EC-A30A-739766328BAF}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>